<commit_message>
Acrescentando alguns dados ao banco de dados (Dump))
</commit_message>
<xml_diff>
--- a/Perguntas e respostas banco de dados.xlsx
+++ b/Perguntas e respostas banco de dados.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb075b8b78035d58/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago.f.santos\Desktop\Anima\Thiago\Aulas\UNA\1 Semestre\Projeto Final\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{F07FA673-6258-4A95-BCC8-E131BECEB515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5A5318B-6537-44E2-AF03-6802D3A2C78C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AC1C116E-25FB-4CDE-977E-CB2619E2B127}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="RESPOSTA" sheetId="1" r:id="rId1"/>
     <sheet name="PERGUNTA" sheetId="2" r:id="rId2"/>
+    <sheet name="TIPO PERGUNTA" sheetId="3" r:id="rId3"/>
+    <sheet name="USUARIO" sheetId="4" r:id="rId4"/>
+    <sheet name="PERSONAGEM" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>Qual das alternativas a seguir NÃO é um tipo de relacionamento?</t>
   </si>
@@ -186,12 +188,72 @@
   </si>
   <si>
     <t>NSERT_PERGUNTA</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Programação</t>
+  </si>
+  <si>
+    <t>Cod_tipo pergunta</t>
+  </si>
+  <si>
+    <t>Pergunta</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>SOBRENOME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>APELIDO</t>
+  </si>
+  <si>
+    <t>SENHA</t>
+  </si>
+  <si>
+    <t>Thiago</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Gladson</t>
+  </si>
+  <si>
+    <t>Ameno</t>
+  </si>
+  <si>
+    <t>Campos</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Gladstone</t>
+  </si>
+  <si>
+    <t>Mandinha</t>
+  </si>
+  <si>
+    <t>Strings Modelo</t>
+  </si>
+  <si>
+    <t>Inserts tabela usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,6 +359,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -643,24 +709,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF8C2C-331C-4ADF-A7FC-6A398D5EBEB0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>44</v>
       </c>
@@ -678,7 +744,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -700,7 +766,7 @@
         <v>(1,1,false),</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -718,11 +784,11 @@
         <v>('Muitos-para-Muitos'),</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F41" si="1">"("&amp;C3&amp;","&amp;D3&amp;","&amp;B3&amp;"),"</f>
+        <f t="shared" ref="F3:F40" si="1">"("&amp;C3&amp;","&amp;D3&amp;","&amp;B3&amp;"),"</f>
         <v>(1,2,false),</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -744,7 +810,7 @@
         <v>(1,3,true),</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -766,7 +832,7 @@
         <v>(1,4,false),</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -788,7 +854,7 @@
         <v>(2,5,true),</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -810,7 +876,7 @@
         <v>(2,6,false),</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -832,7 +898,7 @@
         <v>(2,7,false),</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -854,7 +920,7 @@
         <v>(2,8,false),</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -876,7 +942,7 @@
         <v>(3,9,true),</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -898,7 +964,7 @@
         <v>(3,10,false),</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
@@ -920,7 +986,7 @@
         <v>(3,11,false),</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
@@ -942,7 +1008,7 @@
         <v>(3,12,false),</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -964,7 +1030,7 @@
         <v>(4,13,false),</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -986,7 +1052,7 @@
         <v>(4,14,false),</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -1008,7 +1074,7 @@
         <v>(4,15,true),</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1096,7 @@
         <v>(4,16,false),</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -1052,7 +1118,7 @@
         <v>(5,17,true),</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -1074,7 +1140,7 @@
         <v>(5,18,false),</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -1096,7 +1162,7 @@
         <v>(5,19,false),</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1184,7 @@
         <v>(5,20,false),</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -1140,7 +1206,7 @@
         <v>(6,21,false),</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>29</v>
       </c>
@@ -1162,7 +1228,7 @@
         <v>(6,22,false),</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -1184,7 +1250,7 @@
         <v>(6,23,true),</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>31</v>
       </c>
@@ -1206,7 +1272,7 @@
         <v>(6,24,false),</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>28</v>
       </c>
@@ -1228,7 +1294,7 @@
         <v>(7,25,false),</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
@@ -1250,7 +1316,7 @@
         <v>(7,26,true),</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
@@ -1272,7 +1338,7 @@
         <v>(7,27,false),</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>31</v>
       </c>
@@ -1294,7 +1360,7 @@
         <v>(7,28,false),</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
@@ -1316,7 +1382,7 @@
         <v>(8,29,true),</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
@@ -1338,7 +1404,7 @@
         <v>(8,30,false),</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
@@ -1360,7 +1426,7 @@
         <v>(8,31,false),</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
@@ -1382,7 +1448,7 @@
         <v>(8,32,false),</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>35</v>
       </c>
@@ -1404,7 +1470,7 @@
         <v>(9,33,true),</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>36</v>
       </c>
@@ -1426,7 +1492,7 @@
         <v>(9,34,false),</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>37</v>
       </c>
@@ -1448,7 +1514,7 @@
         <v>(9,35,false),</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>38</v>
       </c>
@@ -1470,7 +1536,7 @@
         <v>(9,36,false),</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>40</v>
       </c>
@@ -1492,7 +1558,7 @@
         <v>(10,37,false),</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>41</v>
       </c>
@@ -1514,7 +1580,7 @@
         <v>(10,38,false),</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>42</v>
       </c>
@@ -1536,7 +1602,7 @@
         <v>(10,39,true),</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>43</v>
       </c>
@@ -1578,21 +1644,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D573898-9F98-4D65-A1A9-C1EC3984E47C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="203.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="203.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -1603,7 +1669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1681,7 @@
         <v>('Qual das alternativas a seguir NÃO é um tipo de relacionamento?',1),</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1627,7 +1693,7 @@
         <v>('Qual das funções a seguir pode ser usada apenas com valores numéricos? ',2),</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1639,7 +1705,7 @@
         <v>('Qual é a maneira mais rápida de acessar uma linha em uma tabela?',1),</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -1651,7 +1717,7 @@
         <v>('Qual das opções abaixo não e uma IDE:',3),</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +1729,7 @@
         <v>('Em Java, a estrutura de repetição que permite que um conjunto de instruções não seja executada nenhuma vez é representada por',2),</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
@@ -1675,7 +1741,7 @@
         <v>('Referente a afirmativa a seguir selecione a alternativa que se encaixa em um significado de metodo JAVA:  "O metodo é visivel apenas pela própria classe. É o qualificador mais restritivo"',2),</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1687,7 +1753,7 @@
         <v>('Referente a afirmativa a seguir selecione a alternativa que se encaixa em um significado de metodo JAVA:  "O metodo  é visível pela própria classe, por suas subclasses e pelas classes do mesmo pacote"',2),</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -1699,7 +1765,7 @@
         <v>('Referente a afirmativa a seguir selecione a alternativa que se encaixa em um significado de metodo JAVA:  "O metodo é visível por qualquer classe, sendo o qualificador mais aberto no sentido de que qualquer classe pode usar esse método"',2),</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -1711,7 +1777,7 @@
         <v>('Qual dos metodos a seguir e utilizado em java para "Imprimir" uma mensagem na tela?',2),</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -1732,4 +1798,748 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF($A2="","","('"&amp;B2&amp;"')")</f>
+        <v>('Banco de dados')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C4" si="0">IF($A3="","","('"&amp;B3&amp;"')")</f>
+        <v>('Java')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>('Programação')</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="50.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LOWER(LEFT(A2,1)&amp;LEFT(B2,1)&amp;"@gmail.com")</f>
+        <v>ts@gmail.com</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF($A2="","","('"&amp;A2&amp;"',")</f>
+        <v>('Thiago',</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G3" si="0">IF($A2="","","'"&amp;B2&amp;"',")</f>
+        <v>'Santos',</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H3" si="1">IF($A2="","","'"&amp;C2&amp;"',")</f>
+        <v>'ts@gmail.com',</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I3" si="2">IF($A2="","","'"&amp;D2&amp;"',")</f>
+        <v>'Thiago',</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF($A2="","","'"&amp;E2&amp;"',),")</f>
+        <v>'123',),</v>
+      </c>
+      <c r="K2" t="str">
+        <f>CONCATENATE(F2,G2,H2,I2,J2)</f>
+        <v>('Thiago','Santos','ts@gmail.com','Thiago','123',),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="str">
+        <f>LOWER(LEFT(A3,1)&amp;LEFT(B3,1)&amp;"@gmail.com")</f>
+        <v>ga@gmail.com</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3">
+        <v>456</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F23" si="3">IF($A3="","","('"&amp;A3&amp;"',")</f>
+        <v>('Gladson',</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>'Ameno',</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="1"/>
+        <v>'ga@gmail.com',</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="2"/>
+        <v>'Gladstone',</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J23" si="4">IF($A3="","","'"&amp;E3&amp;"',),")</f>
+        <v>'456',),</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K23" si="5">CONCATENATE(F3,G3,H3,I3,J3)</f>
+        <v>('Gladson','Ameno','ga@gmail.com','Gladstone','456',),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="str">
+        <f>LOWER(LEFT(A4,1)&amp;LEFT(B4,1)&amp;"@gmail.com")</f>
+        <v>ac@gmail.com</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4">
+        <v>789</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>('Amanda',</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4" si="6">IF($A4="","","'"&amp;B4&amp;"',")</f>
+        <v>'Campos',</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4" si="7">IF($A4="","","'"&amp;C4&amp;"',")</f>
+        <v>'ac@gmail.com',</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4" si="8">IF($A4="","","'"&amp;D4&amp;"',")</f>
+        <v>'Mandinha',</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="4"/>
+        <v>'789',),</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="5"/>
+        <v>('Amanda','Campos','ac@gmail.com','Mandinha','789',),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:I5" si="9">IF($A5="","","'"&amp;B5&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6:G23" si="10">IF($A6="","","'"&amp;B6&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H23" si="11">IF($A6="","","'"&amp;C6&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ref="I6:I23" si="12">IF($A6="","","'"&amp;D6&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Perguntas e respostas banco de dados.xlsx
</commit_message>
<xml_diff>
--- a/Perguntas e respostas banco de dados.xlsx
+++ b/Perguntas e respostas banco de dados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RESPOSTA" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>Qual das alternativas a seguir NÃO é um tipo de relacionamento?</t>
   </si>
@@ -181,15 +181,9 @@
     <t>INSERT_RESPOSTA</t>
   </si>
   <si>
-    <t>INSERT_PERGUNTA_RESPOSTA</t>
-  </si>
-  <si>
     <t>PERGUNTA</t>
   </si>
   <si>
-    <t>NSERT_PERGUNTA</t>
-  </si>
-  <si>
     <t>Banco de dados</t>
   </si>
   <si>
@@ -205,18 +199,9 @@
     <t>Pergunta</t>
   </si>
   <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>SOBRENOME</t>
-  </si>
-  <si>
     <t>EMAIL</t>
   </si>
   <si>
-    <t>APELIDO</t>
-  </si>
-  <si>
     <t>SENHA</t>
   </si>
   <si>
@@ -244,17 +229,35 @@
     <t>Mandinha</t>
   </si>
   <si>
-    <t>Strings Modelo</t>
-  </si>
-  <si>
     <t>Inserts tabela usuario</t>
+  </si>
+  <si>
+    <t>NOME_USUARIO</t>
+  </si>
+  <si>
+    <t>SOBRENOME_USUARIO</t>
+  </si>
+  <si>
+    <t>APELIDO_USUARIO</t>
+  </si>
+  <si>
+    <t>(DESC_PERGUNTA) VALUES</t>
+  </si>
+  <si>
+    <t>(PERGUNTA,COD_TIPO_PERGUNTA) VALUES</t>
+  </si>
+  <si>
+    <t>IND_RESPOSTA_CORRETA</t>
+  </si>
+  <si>
+    <t>ts@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +269,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,13 +376,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,11 +747,13 @@
     <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="C1" t="s">
         <v>46</v>
       </c>
@@ -740,8 +763,9 @@
       <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
-        <v>48</v>
+      <c r="F1" t="str">
+        <f>"("&amp;C1&amp;","&amp;D1&amp;","&amp;B1&amp;") VALUES"</f>
+        <v>(COD_PERGUNTA,COD_RESPOSTA,IND_RESPOSTA_CORRETA) VALUES</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,9 +1649,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>#REF!</formula>
@@ -1647,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,13 +1681,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
+      <c r="C1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,7 +1826,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,10 +1837,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,11 +1851,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="str">
-        <f>IF($A2="","","('"&amp;B2&amp;"')")</f>
-        <v>('Banco de dados')</v>
+        <f>IF($A2="","","('"&amp;B2&amp;"'),")</f>
+        <v>('Banco de dados'),</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,11 +1863,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C4" si="0">IF($A3="","","('"&amp;B3&amp;"')")</f>
-        <v>('Java')</v>
+        <f>IF($A3="","","('"&amp;B3&amp;"'),")</f>
+        <v>('Java'),</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1851,682 +1875,703 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C3:C4" si="0">IF($A4="","","('"&amp;B4&amp;"')")</f>
         <v>('Programação')</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="50.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="str">
-        <f>LOWER(LEFT(A2,1)&amp;LEFT(B2,1)&amp;"@gmail.com")</f>
-        <v>ts@gmail.com</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2">
-        <v>123</v>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K1" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="F2" t="str">
-        <f>IF($A2="","","('"&amp;A2&amp;"',")</f>
-        <v>('Thiago',</v>
-      </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G3" si="0">IF($A2="","","'"&amp;B2&amp;"',")</f>
-        <v>'Santos',</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ref="H2:H3" si="1">IF($A2="","","'"&amp;C2&amp;"',")</f>
-        <v>'ts@gmail.com',</v>
-      </c>
-      <c r="I2" t="str">
-        <f t="shared" ref="I2:I3" si="2">IF($A2="","","'"&amp;D2&amp;"',")</f>
-        <v>'Thiago',</v>
-      </c>
-      <c r="J2" t="str">
-        <f>IF($A2="","","'"&amp;E2&amp;"',),")</f>
-        <v>'123',),</v>
+        <f>IF($A2="","","("&amp;A2&amp;", ")</f>
+        <v xml:space="preserve">(NOME_USUARIO, </v>
+      </c>
+      <c r="G2" s="14" t="str">
+        <f>B2&amp;", "</f>
+        <v xml:space="preserve">SOBRENOME_USUARIO, </v>
+      </c>
+      <c r="H2" s="14" t="str">
+        <f t="shared" ref="H2:I2" si="0">C2&amp;", "</f>
+        <v xml:space="preserve">EMAIL, </v>
+      </c>
+      <c r="I2" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">APELIDO_USUARIO, </v>
+      </c>
+      <c r="J2" s="14" t="str">
+        <f>E2&amp;") VALUES"</f>
+        <v>SENHA) VALUES</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE(F2,G2,H2,I2,J2)</f>
-        <v>('Thiago','Santos','ts@gmail.com','Thiago','123',),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>63</v>
+        <v>(NOME_USUARIO, SOBRENOME_USUARIO, EMAIL, APELIDO_USUARIO, SENHA) VALUES</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3" t="str">
         <f>LOWER(LEFT(A3,1)&amp;LEFT(B3,1)&amp;"@gmail.com")</f>
-        <v>ga@gmail.com</v>
+        <v>ts@gmail.com</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E3">
-        <v>456</v>
+        <v>123</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F23" si="3">IF($A3="","","('"&amp;A3&amp;"',")</f>
-        <v>('Gladson',</v>
+        <f>IF($A3="","","('"&amp;A3&amp;"',")</f>
+        <v>('Thiago',</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>'Ameno',</v>
+        <f t="shared" ref="G3:G4" si="1">IF($A3="","","'"&amp;B3&amp;"',")</f>
+        <v>'Santos',</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" si="1"/>
-        <v>'ga@gmail.com',</v>
+        <f t="shared" ref="H3:H4" si="2">IF($A3="","","'"&amp;C3&amp;"',")</f>
+        <v>'ts@gmail.com',</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="2"/>
-        <v>'Gladstone',</v>
+        <f t="shared" ref="I3:I4" si="3">IF($A3="","","'"&amp;D3&amp;"',")</f>
+        <v>'Thiago',</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J23" si="4">IF($A3="","","'"&amp;E3&amp;"',),")</f>
-        <v>'456',),</v>
+        <f>IF($A3="","","'"&amp;E3&amp;"'),")</f>
+        <v>'123'),</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K23" si="5">CONCATENATE(F3,G3,H3,I3,J3)</f>
-        <v>('Gladson','Ameno','ga@gmail.com','Gladstone','456',),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <f>CONCATENATE(F3,G3,H3,I3,J3)</f>
+        <v>('Thiago','Santos','ts@gmail.com','Thiago','123'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" t="str">
         <f>LOWER(LEFT(A4,1)&amp;LEFT(B4,1)&amp;"@gmail.com")</f>
+        <v>ga@gmail.com</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>456</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F24" si="4">IF($A4="","","('"&amp;A4&amp;"',")</f>
+        <v>('Gladson',</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>'Ameno',</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>'ga@gmail.com',</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="3"/>
+        <v>'Gladstone',</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J24" si="5">IF($A4="","","'"&amp;E4&amp;"'),")</f>
+        <v>'456'),</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K24" si="6">CONCATENATE(F4,G4,H4,I4,J4)</f>
+        <v>('Gladson','Ameno','ga@gmail.com','Gladstone','456'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="str">
+        <f>LOWER(LEFT(A5,1)&amp;LEFT(B5,1)&amp;"@gmail.com")</f>
         <v>ac@gmail.com</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4">
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
         <v>789</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="3"/>
+      <c r="F5" t="str">
+        <f t="shared" si="4"/>
         <v>('Amanda',</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" ref="G4" si="6">IF($A4="","","'"&amp;B4&amp;"',")</f>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5" si="7">IF($A5="","","'"&amp;B5&amp;"',")</f>
         <v>'Campos',</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" ref="H4" si="7">IF($A4="","","'"&amp;C4&amp;"',")</f>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5" si="8">IF($A5="","","'"&amp;C5&amp;"',")</f>
         <v>'ac@gmail.com',</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" ref="I4" si="8">IF($A4="","","'"&amp;D4&amp;"',")</f>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5" si="9">IF($A5="","","'"&amp;D5&amp;"',")</f>
         <v>'Mandinha',</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J5" t="str">
+        <f t="shared" si="5"/>
+        <v>'789'),</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="6"/>
+        <v>('Amanda','Campos','ac@gmail.com','Mandinha','789'),</v>
+      </c>
+      <c r="N5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
         <f t="shared" si="4"/>
-        <v>'789',),</v>
-      </c>
-      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6:I6" si="10">IF($A6="","","'"&amp;B6&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J6" t="str">
         <f t="shared" si="5"/>
-        <v>('Amanda','Campos','ac@gmail.com','Mandinha','789',),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F5" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" ref="G5:I5" si="9">IF($A5="","","'"&amp;B5&amp;"',")</f>
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K5" t="str">
+      <c r="G7" t="str">
+        <f t="shared" ref="G7:G24" si="11">IF($A7="","","'"&amp;B7&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ref="H7:H24" si="12">IF($A7="","","'"&amp;C7&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" ref="I7:I24" si="13">IF($A7="","","'"&amp;D7&amp;"',")</f>
+        <v/>
+      </c>
+      <c r="J7" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" ref="G6:G23" si="10">IF($A6="","","'"&amp;B6&amp;"',")</f>
-        <v/>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" ref="H6:H23" si="11">IF($A6="","","'"&amp;C6&amp;"',")</f>
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" ref="I6:I23" si="12">IF($A6="","","'"&amp;D6&amp;"',")</f>
-        <v/>
-      </c>
-      <c r="J6" t="str">
+      <c r="K7" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K6" t="str">
+      <c r="G8" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F7" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H7" t="str">
+      <c r="K8" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="I7" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="J7" t="str">
+      <c r="I9" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K7" t="str">
+      <c r="G10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J10" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H8" t="str">
+      <c r="K10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G11" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="I8" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="J8" t="str">
+      <c r="I11" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K8" t="str">
+      <c r="G12" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H9" t="str">
+      <c r="K12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G13" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="I9" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="J9" t="str">
+      <c r="I13" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K9" t="str">
+      <c r="G14" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J14" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H10" t="str">
+      <c r="K14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G15" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="I10" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="J10" t="str">
+      <c r="I15" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K10" t="str">
+      <c r="G16" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J16" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F14" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K15" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H23" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G24" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="I23" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="J23" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K23" t="str">
+      <c r="I24" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J24" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
+      <c r="K24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:J1"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Insertes personagem e Habilidades e Update planilha excel
</commit_message>
<xml_diff>
--- a/Perguntas e respostas banco de dados.xlsx
+++ b/Perguntas e respostas banco de dados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago.f.santos\Desktop\Anima\Thiago\Aulas\UNA\1 Semestre\Projeto Final\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faculdade\Projeto\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0D16D6-D48D-4DFC-807E-605AF5218A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESPOSTA" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,9 @@
     <sheet name="TIPO PERGUNTA" sheetId="3" r:id="rId3"/>
     <sheet name="USUARIO" sheetId="4" r:id="rId4"/>
     <sheet name="PERSONAGEM" sheetId="5" r:id="rId5"/>
+    <sheet name="HABILIDADES" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
     <t>Qual das alternativas a seguir NÃO é um tipo de relacionamento?</t>
   </si>
@@ -251,12 +253,75 @@
   </si>
   <si>
     <t>ts@gmail.com</t>
+  </si>
+  <si>
+    <t>cod personagem</t>
+  </si>
+  <si>
+    <t>nome personagem</t>
+  </si>
+  <si>
+    <t>Naruto</t>
+  </si>
+  <si>
+    <t>Boruto</t>
+  </si>
+  <si>
+    <t>Sonic</t>
+  </si>
+  <si>
+    <t>Deku</t>
+  </si>
+  <si>
+    <t>Saitama</t>
+  </si>
+  <si>
+    <t>cod habilidade</t>
+  </si>
+  <si>
+    <t>desc habilidade</t>
+  </si>
+  <si>
+    <t>Sair do jogo sem perder vida</t>
+  </si>
+  <si>
+    <t>Retirar 10pts do Adversario</t>
+  </si>
+  <si>
+    <t>Duplicar o valor de pts da pergunta</t>
+  </si>
+  <si>
+    <t>Retirar pontos de vida de Adversario</t>
+  </si>
+  <si>
+    <t>Pular pergunta</t>
+  </si>
+  <si>
+    <t>Ganhar 10 de vida</t>
+  </si>
+  <si>
+    <t>Ganhar 20 de vida</t>
+  </si>
+  <si>
+    <t>Perder 10 de vida e ganhar 10 pontos</t>
+  </si>
+  <si>
+    <t>Perder 20 pontos e ganhar 20 de vida</t>
+  </si>
+  <si>
+    <t>Modo Deus</t>
+  </si>
+  <si>
+    <t>COD_PERSONAGEM</t>
+  </si>
+  <si>
+    <t>(desc habilidade,cod_personagem) VALUES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -730,24 +795,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F41"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.109375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
@@ -763,12 +828,12 @@
       <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="str">
+      <c r="F1" s="10" t="str">
         <f>"("&amp;C1&amp;","&amp;D1&amp;","&amp;B1&amp;") VALUES"</f>
         <v>(COD_PERGUNTA,COD_RESPOSTA,IND_RESPOSTA_CORRETA) VALUES</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -785,12 +850,12 @@
         <f>"('"&amp;A2&amp;"'),"</f>
         <v>('Um-para-Muitos'),</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F2" s="10" t="str">
         <f>"("&amp;C2&amp;","&amp;D2&amp;","&amp;B2&amp;"),"</f>
         <v>(1,1,false),</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -807,12 +872,12 @@
         <f t="shared" ref="E3:E41" si="0">"('"&amp;A3&amp;"'),"</f>
         <v>('Muitos-para-Muitos'),</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F3" s="10" t="str">
         <f t="shared" ref="F3:F40" si="1">"("&amp;C3&amp;","&amp;D3&amp;","&amp;B3&amp;"),"</f>
         <v>(1,2,false),</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -829,12 +894,12 @@
         <f t="shared" si="0"/>
         <v>('Algum-para-Nenhum'),</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(1,3,true),</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -851,12 +916,12 @@
         <f t="shared" si="0"/>
         <v>('Um-para-Um'),</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(1,4,false),</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -873,12 +938,12 @@
         <f t="shared" si="0"/>
         <v>('SUM'),</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(2,5,true),</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -895,12 +960,12 @@
         <f t="shared" si="0"/>
         <v>('INSERT'),</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(2,6,false),</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -917,12 +982,12 @@
         <f t="shared" si="0"/>
         <v>('UPDATE'),</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F8" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(2,7,false),</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -939,12 +1004,12 @@
         <f t="shared" si="0"/>
         <v>('CREATE'),</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F9" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(2,8,false),</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -961,12 +1026,12 @@
         <f t="shared" si="0"/>
         <v>('Usando o ROWID'),</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F10" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(3,9,true),</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -983,12 +1048,12 @@
         <f t="shared" si="0"/>
         <v>('Usando o UPDATE'),</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(3,10,false),</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
@@ -1005,12 +1070,12 @@
         <f t="shared" si="0"/>
         <v>('Usando o SUM'),</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F12" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(3,11,false),</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
@@ -1027,12 +1092,12 @@
         <f t="shared" si="0"/>
         <v>('Usando o INSERT'),</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(3,12,false),</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1049,12 +1114,12 @@
         <f t="shared" si="0"/>
         <v>('NetBeans'),</v>
       </c>
-      <c r="F14" t="str">
+      <c r="F14" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(4,13,false),</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1071,12 +1136,12 @@
         <f t="shared" si="0"/>
         <v>('Eclipse'),</v>
       </c>
-      <c r="F15" t="str">
+      <c r="F15" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(4,14,false),</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -1093,12 +1158,12 @@
         <f t="shared" si="0"/>
         <v>('Windows XP'),</v>
       </c>
-      <c r="F16" t="str">
+      <c r="F16" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(4,15,true),</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
@@ -1115,12 +1180,12 @@
         <f t="shared" si="0"/>
         <v>('Dr. Java'),</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F17" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(4,16,false),</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -1137,12 +1202,12 @@
         <f t="shared" si="0"/>
         <v>('While'),</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F18" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(5,17,true),</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -1159,12 +1224,12 @@
         <f t="shared" si="0"/>
         <v>('Switch'),</v>
       </c>
-      <c r="F19" t="str">
+      <c r="F19" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(5,18,false),</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -1181,12 +1246,12 @@
         <f t="shared" si="0"/>
         <v>('Case'),</v>
       </c>
-      <c r="F20" t="str">
+      <c r="F20" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(5,19,false),</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>26</v>
       </c>
@@ -1203,12 +1268,12 @@
         <f t="shared" si="0"/>
         <v>('Continue'),</v>
       </c>
-      <c r="F21" t="str">
+      <c r="F21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(5,20,false),</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -1225,12 +1290,12 @@
         <f t="shared" si="0"/>
         <v>('Public'),</v>
       </c>
-      <c r="F22" t="str">
+      <c r="F22" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(6,21,false),</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>29</v>
       </c>
@@ -1247,12 +1312,12 @@
         <f t="shared" si="0"/>
         <v>('Protected'),</v>
       </c>
-      <c r="F23" t="str">
+      <c r="F23" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(6,22,false),</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -1269,12 +1334,12 @@
         <f t="shared" si="0"/>
         <v>('Private'),</v>
       </c>
-      <c r="F24" t="str">
+      <c r="F24" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(6,23,true),</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>31</v>
       </c>
@@ -1291,12 +1356,12 @@
         <f t="shared" si="0"/>
         <v>('Nenhuma das alternativas'),</v>
       </c>
-      <c r="F25" t="str">
+      <c r="F25" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(6,24,false),</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>28</v>
       </c>
@@ -1313,12 +1378,12 @@
         <f t="shared" si="0"/>
         <v>('Public'),</v>
       </c>
-      <c r="F26" t="str">
+      <c r="F26" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(7,25,false),</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
@@ -1335,12 +1400,12 @@
         <f t="shared" si="0"/>
         <v>('Protected'),</v>
       </c>
-      <c r="F27" t="str">
+      <c r="F27" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(7,26,true),</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
@@ -1357,12 +1422,12 @@
         <f t="shared" si="0"/>
         <v>('Private'),</v>
       </c>
-      <c r="F28" t="str">
+      <c r="F28" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(7,27,false),</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>31</v>
       </c>
@@ -1379,12 +1444,12 @@
         <f t="shared" si="0"/>
         <v>('Nenhuma das alternativas'),</v>
       </c>
-      <c r="F29" t="str">
+      <c r="F29" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(7,28,false),</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
@@ -1401,12 +1466,12 @@
         <f t="shared" si="0"/>
         <v>('Public'),</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F30" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(8,29,true),</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
@@ -1423,12 +1488,12 @@
         <f t="shared" si="0"/>
         <v>('Protected'),</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F31" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(8,30,false),</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
@@ -1445,12 +1510,12 @@
         <f t="shared" si="0"/>
         <v>('Private'),</v>
       </c>
-      <c r="F32" t="str">
+      <c r="F32" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(8,31,false),</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
@@ -1467,12 +1532,12 @@
         <f t="shared" si="0"/>
         <v>('Nenhuma das alternativas'),</v>
       </c>
-      <c r="F33" t="str">
+      <c r="F33" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(8,32,false),</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>35</v>
       </c>
@@ -1489,12 +1554,12 @@
         <f t="shared" si="0"/>
         <v>('System.out.println("Aluma coisa")'),</v>
       </c>
-      <c r="F34" t="str">
+      <c r="F34" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(9,33,true),</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>36</v>
       </c>
@@ -1511,12 +1576,12 @@
         <f t="shared" si="0"/>
         <v>('System.static.println("Aluma coisa")'),</v>
       </c>
-      <c r="F35" t="str">
+      <c r="F35" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(9,34,false),</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>37</v>
       </c>
@@ -1533,12 +1598,12 @@
         <f t="shared" si="0"/>
         <v>('System.out.print("Aluma coisa")'),</v>
       </c>
-      <c r="F36" t="str">
+      <c r="F36" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(9,35,false),</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>38</v>
       </c>
@@ -1555,12 +1620,12 @@
         <f t="shared" si="0"/>
         <v>('Imprimir("Aluma coisa")'),</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F37" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(9,36,false),</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>40</v>
       </c>
@@ -1577,12 +1642,12 @@
         <f t="shared" si="0"/>
         <v>('Importar biblioteca'),</v>
       </c>
-      <c r="F38" t="str">
+      <c r="F38" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(10,37,false),</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>41</v>
       </c>
@@ -1599,12 +1664,12 @@
         <f t="shared" si="0"/>
         <v>('impoting'),</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F39" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(10,38,false),</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>42</v>
       </c>
@@ -1621,12 +1686,12 @@
         <f t="shared" si="0"/>
         <v>('impot'),</v>
       </c>
-      <c r="F40" t="str">
+      <c r="F40" s="10" t="str">
         <f t="shared" si="1"/>
         <v>(10,39,true),</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>43</v>
       </c>
@@ -1643,7 +1708,7 @@
         <f t="shared" si="0"/>
         <v>('import library'),</v>
       </c>
-      <c r="F41" t="str">
+      <c r="F41" s="10" t="str">
         <f>"("&amp;C41&amp;","&amp;D41&amp;","&amp;B41&amp;");"</f>
         <v>(10,40,false);</v>
       </c>
@@ -1665,21 +1730,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="203.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="203.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -1690,7 +1755,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1702,7 +1767,7 @@
         <v>('Qual das alternativas a seguir NÃO é um tipo de relacionamento?',1),</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1779,7 @@
         <v>('Qual das funções a seguir pode ser usada apenas com valores numéricos? ',2),</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1726,7 +1791,7 @@
         <v>('Qual é a maneira mais rápida de acessar uma linha em uma tabela?',1),</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -1738,7 +1803,7 @@
         <v>('Qual das opções abaixo não e uma IDE:',3),</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1750,7 +1815,7 @@
         <v>('Em Java, a estrutura de repetição que permite que um conjunto de instruções não seja executada nenhuma vez é representada por',2),</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
@@ -1762,7 +1827,7 @@
         <v>('Referente a afirmativa a seguir selecione a alternativa que se encaixa em um significado de metodo JAVA:  "O metodo é visivel apenas pela própria classe. É o qualificador mais restritivo"',2),</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1774,7 +1839,7 @@
         <v>('Referente a afirmativa a seguir selecione a alternativa que se encaixa em um significado de metodo JAVA:  "O metodo  é visível pela própria classe, por suas subclasses e pelas classes do mesmo pacote"',2),</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -1786,7 +1851,7 @@
         <v>('Referente a afirmativa a seguir selecione a alternativa que se encaixa em um significado de metodo JAVA:  "O metodo é visível por qualquer classe, sendo o qualificador mais aberto no sentido de que qualquer classe pode usar esse método"',2),</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -1798,7 +1863,7 @@
         <v>('Qual dos metodos a seguir e utilizado em java para "Imprimir" uma mensagem na tela?',2),</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -1822,20 +1887,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1846,7 +1911,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1858,7 +1923,7 @@
         <v>('Banco de dados'),</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1870,7 +1935,7 @@
         <v>('Java'),</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1878,7 +1943,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C3:C4" si="0">IF($A4="","","('"&amp;B4&amp;"')")</f>
+        <f t="shared" ref="C4" si="0">IF($A4="","","('"&amp;B4&amp;"')")</f>
         <v>('Programação')</v>
       </c>
     </row>
@@ -1889,25 +1954,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K1" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="14" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>65</v>
       </c>
@@ -1948,7 +2013,7 @@
         <v>(NOME_USUARIO, SOBRENOME_USUARIO, EMAIL, APELIDO_USUARIO, SENHA) VALUES</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>56</v>
       </c>
@@ -1990,7 +2055,7 @@
         <v>('Thiago','Santos','ts@gmail.com','Thiago','123'),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2032,7 +2097,7 @@
         <v>('Gladson','Ameno','ga@gmail.com','Gladstone','456'),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -2077,7 +2142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F6" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2103,7 +2168,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F7" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2129,7 +2194,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F8" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2155,7 +2220,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F9" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2181,7 +2246,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F10" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2207,7 +2272,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F11" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2233,7 +2298,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2259,7 +2324,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2285,7 +2350,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F14" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2311,7 +2376,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F15" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2337,7 +2402,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2363,7 +2428,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F17" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2389,7 +2454,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F18" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2415,7 +2480,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F19" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2441,7 +2506,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F20" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2467,7 +2532,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F21" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2493,7 +2558,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2519,7 +2584,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F23" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2545,7 +2610,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F24" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2578,13 +2643,272 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF($A2="","","('"&amp;B2&amp;"'),")</f>
+        <v>('Naruto'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="str">
+        <f>IF($A3="","","('"&amp;B3&amp;"'),")</f>
+        <v>('Boruto'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IF($A4="","","('"&amp;B4&amp;"'),")</f>
+        <v>('Sonic'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="str">
+        <f>IF($A5="","","('"&amp;B5&amp;"'),")</f>
+        <v>('Deku'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF($A6="","","('"&amp;B6&amp;"');")</f>
+        <v>('Saitama');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CF001F-6089-4D34-8453-5CBA5F219689}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF($A2="","","('"&amp;B2&amp;"',"&amp;C2&amp;"),")</f>
+        <v>('Sair do jogo sem perder vida',1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D11" si="0">IF($A3="","","('"&amp;B3&amp;"',"&amp;C3&amp;"),")</f>
+        <v>('Retirar 10pts do Adversario',2),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>('Duplicar o valor de pts da pergunta',3),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>('Retirar pontos de vida de Adversario',4),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>('Pular pergunta',5),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>('Ganhar 10 de vida',1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>('Ganhar 20 de vida',2),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>('Perder 10 de vida e ganhar 10 pontos',3),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>('Perder 20 pontos e ganhar 20 de vida',4),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="str">
+        <f>IF($A11="","","('"&amp;B11&amp;"',"&amp;C11&amp;");")</f>
+        <v>('Modo Deus',5);</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>